<commit_message>
change excel column names
</commit_message>
<xml_diff>
--- a/data/Students.xlsx
+++ b/data/Students.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunnyng/Dev/R-Intro/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F51170DF-33B1-F449-875E-DEBD4E22DA20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44D89217-064C-7F4E-BE33-62EFDD2C9F0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="2000" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{B5BC7606-6C6A-B04E-8B14-83FF75E9AE06}"/>
+    <workbookView xWindow="3180" yWindow="2000" windowWidth="27640" windowHeight="16940" xr2:uid="{B5BC7606-6C6A-B04E-8B14-83FF75E9AE06}"/>
   </bookViews>
   <sheets>
     <sheet name="Intake" sheetId="1" r:id="rId1"/>
@@ -35,35 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
-  <si>
-    <t>Academic year</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>Associate Degree</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>Higher Diploma</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sub-degree</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>First year first degree</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>Top-up degree</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>Under-graduate</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
   <si>
     <t>2007/08</t>
     <phoneticPr fontId="0" type="noConversion"/>
@@ -115,34 +87,6 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>Academic year</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Associate Degree</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Higher Diploma</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sub-degree</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>First year first degree</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Top-up degree</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Under-graduate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>2007/08</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -185,6 +129,27 @@
   <si>
     <t>2018/19</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AcademicYear</t>
+  </si>
+  <si>
+    <t>AssociateDegree</t>
+  </si>
+  <si>
+    <t>HigherDiploma</t>
+  </si>
+  <si>
+    <t>Subdegree</t>
+  </si>
+  <si>
+    <t>FirstYearFirstDegree</t>
+  </si>
+  <si>
+    <t>Undergraduate</t>
+  </si>
+  <si>
+    <t>TopUpDegree</t>
   </si>
 </sst>
 </file>
@@ -548,38 +513,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64191412-3DAA-DF41-A88C-60EBDECF5E33}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1">
         <v>12029</v>
@@ -602,7 +567,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1">
         <v>11238</v>
@@ -625,7 +590,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1">
         <v>14177</v>
@@ -648,7 +613,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1">
         <v>17646</v>
@@ -671,7 +636,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1">
         <f>2598+13420</f>
@@ -695,7 +660,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1">
         <f>73+802+17256</f>
@@ -719,7 +684,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1">
         <v>11715</v>
@@ -742,7 +707,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1">
         <v>10275</v>
@@ -765,7 +730,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1">
         <v>10942</v>
@@ -788,7 +753,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B11" s="1">
         <v>11127</v>
@@ -811,7 +776,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1">
         <v>11420</v>
@@ -837,7 +802,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B13" s="1">
         <v>11574</v>
@@ -863,7 +828,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B14" s="1">
         <v>11170</v>
@@ -895,38 +860,46 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1BF73E6-33FE-0F42-8855-C389CC473C91}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1">
         <v>7159</v>
@@ -941,7 +914,7 @@
         <v>1558</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="G2" s="1">
         <v>1558</v>
@@ -949,7 +922,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1">
         <v>7211</v>
@@ -964,7 +937,7 @@
         <v>2065</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="G3" s="1">
         <v>2065</v>
@@ -972,7 +945,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1">
         <v>7303</v>
@@ -995,7 +968,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1">
         <v>8026</v>
@@ -1018,7 +991,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1">
         <v>9468</v>
@@ -1041,7 +1014,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1">
         <v>10541</v>
@@ -1064,7 +1037,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1">
         <v>13035</v>
@@ -1087,7 +1060,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="B9" s="1">
         <v>9061</v>
@@ -1110,7 +1083,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="B10" s="1">
         <v>7962</v>
@@ -1133,7 +1106,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="B11" s="1">
         <v>8246</v>
@@ -1156,7 +1129,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B12" s="1">
         <v>8460</v>
@@ -1181,7 +1154,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="B13" s="1">
         <v>8334</v>

</xml_diff>